<commit_message>
added application icon, Added Hardware STOP message to ensure the pump is STOPPED, Changed the wording of the exit prompt to Save Report or Quit.
</commit_message>
<xml_diff>
--- a/BugReports/BugLog.xlsx
+++ b/BugReports/BugLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00788a1fe100dfc/Documents/GitHub/PWC-OLS/BugReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{98CCDA7E-CD56-4205-BCEA-8664FEB07457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{546DE554-4628-42B5-A244-0C949AA2F909}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{98CCDA7E-CD56-4205-BCEA-8664FEB07457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC1E6A99-BEA5-471C-89CD-8CB33821AC28}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="780" windowWidth="17180" windowHeight="10310" activeTab="1" xr2:uid="{B1E41434-D84E-4F0F-BC7A-8DEAD0687A50}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{B1E41434-D84E-4F0F-BC7A-8DEAD0687A50}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>DAtaQ can blink bluie??  At power up the discret IO was not responding to the Test Tank VI causing the pump to continuously run.  Reboot PC. DataQ blink Yellow and Test Tank VI had control of the pump with DD PWR turned ON.  After some time the DataQ status LED turned RED will working in MS Excel.</t>
+  </si>
+  <si>
+    <t>rsk</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>When stopping the program, the pump continues to run.</t>
+  </si>
+  <si>
+    <t>Start button pressed, fill light on; in jog mode turn fill off and back on (toggling)</t>
   </si>
 </sst>
 </file>
@@ -409,10 +421,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -817,7 +825,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -895,8 +903,45 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G4" s="16"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="13">
+        <v>45454</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="13">
+        <v>45454</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="H4" s="15"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>